<commit_message>
Bug fix for currency conversion
</commit_message>
<xml_diff>
--- a/InputData/web-app/OCCF/Output Currency Conversion Factors.xlsx
+++ b/InputData/web-app/OCCF/Output Currency Conversion Factors.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deept\OneDrive\Desktop\India InputData 5-6-2020\web-app\OCCF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganM\Documents\eps-india\InputData\web-app\OCCF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D12801F-88E5-4A33-8F96-E7FDB5C2404E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,7 @@
     <sheet name="OCCF-DpMOCU" sheetId="4" r:id="rId3"/>
     <sheet name="OCCF-DpSOCU" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
   <si>
     <t>Source:</t>
   </si>
@@ -102,21 +101,6 @@
     <t>Ruppees per dollar</t>
   </si>
   <si>
-    <t>India Inflation Rates</t>
-  </si>
-  <si>
-    <t>http://www.inflation.eu/inflation-rates/india/historic-inflation/cpi-inflation-india.aspx</t>
-  </si>
-  <si>
-    <t>Year</t>
-  </si>
-  <si>
-    <t>Rate</t>
-  </si>
-  <si>
-    <t>Value Indexed to 2012</t>
-  </si>
-  <si>
     <t>Rupees</t>
   </si>
   <si>
@@ -124,12 +108,42 @@
   </si>
   <si>
     <t>Lakhs</t>
+  </si>
+  <si>
+    <t>https://www.poundsterlinglive.com/best-exchange-rates/best-us-dollar-to-indian-rupee-history-2018</t>
+  </si>
+  <si>
+    <t>US Inflation Rate</t>
+  </si>
+  <si>
+    <t>see cpi.xlsx</t>
+  </si>
+  <si>
+    <t>Recall, this variable is "dollars per large/medium/small currency output unit"</t>
+  </si>
+  <si>
+    <t>2012 dollars are worth more than 2018 dollars, so we need a</t>
+  </si>
+  <si>
+    <t>value less than 1 in this variable.</t>
+  </si>
+  <si>
+    <t>This is why we multiply, not divide, by the conversion</t>
+  </si>
+  <si>
+    <t>factor above.</t>
+  </si>
+  <si>
+    <t>which in this case is "2012 dollars per 2018 rupee."</t>
+  </si>
+  <si>
+    <t>2018 to 2012 dollar adjustment</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0E+00"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
@@ -151,9 +165,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <i/>
       <sz val="11"/>
-      <color theme="10"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -182,11 +196,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -199,16 +212,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -300,23 +315,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -352,23 +350,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -544,34 +525,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="26.28515625" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="26.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -579,58 +561,58 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B17" s="6"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" s="9">
         <f>10^7</f>
         <v>10000000</v>
@@ -639,21 +621,21 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" s="9"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B21" s="6"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23">
         <f>10^5</f>
         <v>100000</v>
@@ -662,167 +644,145 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B25" s="6"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A29">
-        <v>2012</v>
+        <v>2018</v>
       </c>
       <c r="B29">
-        <v>54.77</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+        <v>68.492000000000004</v>
+      </c>
+      <c r="C29" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B32" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C32" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>2010</v>
-      </c>
-      <c r="B33" s="12">
-        <v>9.4700000000000006E-2</v>
-      </c>
-      <c r="C33" s="13">
-        <f>C34/(1+B34)</f>
-        <v>0.84470208721577789</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>2011</v>
-      </c>
-      <c r="B34" s="12">
-        <v>6.4899999999999999E-2</v>
-      </c>
-      <c r="C34" s="13">
-        <f>C35/(1+B35)</f>
-        <v>0.8995232526760818</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>2012</v>
-      </c>
-      <c r="B35" s="12">
-        <v>0.11169999999999999</v>
-      </c>
-      <c r="C35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>2013</v>
-      </c>
-      <c r="B36" s="12">
-        <v>9.1300000000000006E-2</v>
-      </c>
-      <c r="C36" s="13">
-        <f>C35*(1+B36)</f>
-        <v>1.0912999999999999</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>2014</v>
-      </c>
-      <c r="B37" s="12">
-        <v>5.8599999999999999E-2</v>
-      </c>
-      <c r="C37" s="13">
-        <f t="shared" ref="C37:C41" si="0">C36*(1+B37)</f>
-        <v>1.1552501799999999</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>2015</v>
-      </c>
-      <c r="B38" s="12">
-        <v>6.3200000000000006E-2</v>
-      </c>
-      <c r="C38" s="13">
-        <f t="shared" si="0"/>
-        <v>1.2282619913759998</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>2016</v>
-      </c>
-      <c r="B39" s="12">
-        <v>2.23E-2</v>
-      </c>
-      <c r="C39" s="13">
-        <f t="shared" si="0"/>
-        <v>1.2556522337836846</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>2017</v>
-      </c>
-      <c r="B40" s="14">
-        <v>0.04</v>
-      </c>
-      <c r="C40" s="13">
-        <f t="shared" si="0"/>
-        <v>1.3058783231350322</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>2018</v>
-      </c>
-      <c r="B41" s="12">
-        <v>5.2400000000000002E-2</v>
-      </c>
-      <c r="C41" s="13">
-        <f t="shared" si="0"/>
-        <v>1.3743063472673078</v>
-      </c>
+      <c r="B31" s="15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A32" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="10">
+        <v>0.9143273584567535</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B33" s="11"/>
+      <c r="C33" s="12"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
+        <v>29</v>
+      </c>
+      <c r="B34" s="11"/>
+      <c r="C34" s="12"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" s="11"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
+        <v>30</v>
+      </c>
+      <c r="B36" s="11"/>
+      <c r="C36" s="12"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
+        <v>31</v>
+      </c>
+      <c r="B37" s="11"/>
+      <c r="C37" s="12"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
+        <v>32</v>
+      </c>
+      <c r="B38" s="11"/>
+      <c r="C38" s="12"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B39" s="11"/>
+      <c r="C39" s="12"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B40" s="13"/>
+      <c r="C40" s="12"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B41" s="11"/>
+      <c r="C41" s="12"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C31" r:id="rId1" xr:uid="{12F3B7ED-D5E6-4629-877E-19C50DE02103}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="3"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="31.265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B1" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="3">
+        <f>About!A19/About!B29*About!B32</f>
+        <v>133494.03703450819</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -832,23 +792,23 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+    <col min="2" max="2" width="31.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B1" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="3">
-        <f>About!A19/About!B29*About!C41</f>
-        <v>250923.19650672041</v>
+        <v>23</v>
+      </c>
+      <c r="B2" s="8">
+        <f>About!A23/About!B29*About!B32</f>
+        <v>1334.9403703450819</v>
       </c>
     </row>
   </sheetData>
@@ -856,8 +816,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -867,58 +827,23 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+    <col min="2" max="2" width="31.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B1" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="8">
-        <f>About!A23/About!B29*About!C41</f>
-        <v>2509.2319650672043</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <sheetPr>
-    <tabColor theme="3"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="31.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B1" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B2" s="7">
-        <f>1/About!B29*About!C41</f>
-        <v>2.5092319650672042E-2</v>
+        <f>1/About!B29*About!B32</f>
+        <v>1.3349403703450818E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
WRI requested web app edits
</commit_message>
<xml_diff>
--- a/InputData/web-app/OCCF/Output Currency Conversion Factors.xlsx
+++ b/InputData/web-app/OCCF/Output Currency Conversion Factors.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganM\Documents\eps-india\InputData\web-app\OCCF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-india\InputData\web-app\OCCF\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CA9F84F-F18F-4E0A-B715-EF9283B2163A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -17,12 +18,15 @@
     <sheet name="OCCF-DpMOCU" sheetId="4" r:id="rId3"/>
     <sheet name="OCCF-DpSOCU" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -83,12 +87,6 @@
     <t>For the India model:</t>
   </si>
   <si>
-    <t>2018 crores</t>
-  </si>
-  <si>
-    <t>rupees per crore</t>
-  </si>
-  <si>
     <t>2018 lakhs</t>
   </si>
   <si>
@@ -138,12 +136,18 @@
   </si>
   <si>
     <t>2018 to 2012 dollar adjustment</t>
+  </si>
+  <si>
+    <t>2018 lakh crores</t>
+  </si>
+  <si>
+    <t>rupees per lakh crore</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0E+00"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
@@ -315,6 +319,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -350,6 +371,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -525,35 +563,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" customWidth="1"/>
-    <col min="2" max="2" width="26.265625" customWidth="1"/>
+    <col min="1" max="1" width="16.36328125" customWidth="1"/>
+    <col min="2" max="2" width="26.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -561,106 +599,106 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B17" s="6"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="9">
-        <f>10^7</f>
-        <v>10000000</v>
+        <f>10^7*10^5</f>
+        <v>1000000000000</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="9"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B21" s="6"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23">
         <f>10^5</f>
         <v>100000</v>
       </c>
       <c r="B23" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B25" s="6"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>2018</v>
       </c>
@@ -668,75 +706,75 @@
         <v>68.492000000000004</v>
       </c>
       <c r="C29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B31" s="15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A31" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B31" s="15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B32" s="10">
         <v>0.9143273584567535</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B33" s="11"/>
       <c r="C33" s="12"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B34" s="11"/>
       <c r="C34" s="12"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B35" s="11"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B36" s="11"/>
       <c r="C36" s="12"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B37" s="11"/>
       <c r="C37" s="12"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B38" s="11"/>
       <c r="C38" s="12"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B39" s="11"/>
       <c r="C39" s="12"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B40" s="13"/>
       <c r="C40" s="12"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B41" s="11"/>
       <c r="C41" s="12"/>
     </row>
@@ -747,42 +785,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor theme="3"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="2" max="2" width="31.265625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B1" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="3">
-        <f>About!A19/About!B29*About!B32</f>
-        <v>133494.03703450819</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -792,23 +795,23 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="31.265625" customWidth="1"/>
+    <col min="2" max="2" width="31.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B1" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="8">
-        <f>About!A23/About!B29*About!B32</f>
-        <v>1334.9403703450819</v>
+        <v>21</v>
+      </c>
+      <c r="B2" s="3">
+        <f>About!A19/About!B29*About!B32</f>
+        <v>13349403703.450817</v>
       </c>
     </row>
   </sheetData>
@@ -816,8 +819,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -827,19 +830,54 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="31.265625" customWidth="1"/>
+    <col min="2" max="2" width="31.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B1" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="8">
+        <f>About!A23/About!B29*About!B32</f>
+        <v>1334.9403703450819</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <sheetPr>
+    <tabColor theme="3"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="31.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B1" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B2" s="7">
         <f>1/About!B29*About!B32</f>

</xml_diff>